<commit_message>
Comprehensive Test Execution Trends
</commit_message>
<xml_diff>
--- a/inputs/test_suite.xlsx
+++ b/inputs/test_suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProjects\cross_db_validator\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F1B66C-E3F7-474A-A7DE-618F956EDCF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C7D451-1E92-45D8-A865-1824435B94BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTROLLER" sheetId="2" r:id="rId1"/>
@@ -458,9 +458,6 @@
     <t>schema,validation,products</t>
   </si>
   <si>
-    <t>source_table=products;target_table=new_products;ignore_sequence=true;check_constraints=true</t>
-  </si>
-  <si>
     <t>DVAL_002</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>schema,validation,employees</t>
   </si>
   <si>
-    <t>source_table=employees;target_table=new_employees;ignore_sequence=true;check_constraints=true</t>
-  </si>
-  <si>
     <t>DVAL_003</t>
   </si>
   <si>
@@ -488,9 +482,6 @@
     <t>schema,validation,orders</t>
   </si>
   <si>
-    <t>source_table=orders;target_table=new_orders;ignore_sequence=true;check_constraints=true</t>
-  </si>
-  <si>
     <t>DVAL_004</t>
   </si>
   <si>
@@ -509,9 +500,6 @@
     <t>count,validation,products</t>
   </si>
   <si>
-    <t>source_table=products;target_table=new_products;tolerance_percent=5;expected_variance=large</t>
-  </si>
-  <si>
     <t>DVAL_005</t>
   </si>
   <si>
@@ -524,9 +512,6 @@
     <t>count,validation,employees</t>
   </si>
   <si>
-    <t>source_table=employees;target_table=new_employees;tolerance_percent=5;expected_variance=large</t>
-  </si>
-  <si>
     <t>DVAL_006</t>
   </si>
   <si>
@@ -539,9 +524,6 @@
     <t>count,validation,orders</t>
   </si>
   <si>
-    <t>source_table=orders;target_table=new_orders;tolerance_percent=5;expected_variance=large</t>
-  </si>
-  <si>
     <t>DVAL_007</t>
   </si>
   <si>
@@ -560,9 +542,6 @@
     <t>null,validation,products</t>
   </si>
   <si>
-    <t>source_table=products;target_table=new_products;null_match_required=false;report_differences=true</t>
-  </si>
-  <si>
     <t>DVAL_008</t>
   </si>
   <si>
@@ -575,9 +554,6 @@
     <t>null,validation,employees</t>
   </si>
   <si>
-    <t>source_table=employees;target_table=new_employees;null_match_required=false;report_differences=true</t>
-  </si>
-  <si>
     <t>DVAL_009</t>
   </si>
   <si>
@@ -590,9 +566,6 @@
     <t>null,validation,orders</t>
   </si>
   <si>
-    <t>source_table=orders;target_table=new_orders;null_match_required=false;report_differences=true</t>
-  </si>
-  <si>
     <t>ENHANCED UNIFIED SDM TEST SUITE - COMPREHENSIVE INSTRUCTIONS</t>
   </si>
   <si>
@@ -1503,6 +1476,33 @@
   </si>
   <si>
     <t>COL_COL_VALIDATION</t>
+  </si>
+  <si>
+    <t>source_table=public.products;target_table=public.new_products;ignore_sequence=true;check_constraints=true</t>
+  </si>
+  <si>
+    <t>source_table=public.employees;target_table=public.new_employees;ignore_sequence=true;check_constraints=true</t>
+  </si>
+  <si>
+    <t>source_table=public.orders;target_table=public.new_orders;ignore_sequence=true;check_constraints=true</t>
+  </si>
+  <si>
+    <t>source_table=public.products;target_table=public.new_products;tolerance_percent=5;expected_variance=large</t>
+  </si>
+  <si>
+    <t>source_table=public.employees;target_table=public.new_employees;tolerance_percent=5;expected_variance=large</t>
+  </si>
+  <si>
+    <t>source_table=public.orders;target_table=public.new_orders;tolerance_percent=5;expected_variance=large</t>
+  </si>
+  <si>
+    <t>source_table=public.products;target_table=public.new_products;null_match_required=false;report_differences=true</t>
+  </si>
+  <si>
+    <t>source_table=public.employees;target_table=public.new_employees;null_match_required=false;report_differences=true</t>
+  </si>
+  <si>
+    <t>source_table=public.orders;target_table=public.new_orders;null_match_required=false;report_differences=true</t>
   </si>
 </sst>
 </file>
@@ -2035,13 +2035,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -2052,7 +2052,7 @@
         <v>134</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2063,7 +2063,7 @@
         <v>137</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -2080,8 +2080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3287,8 +3287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3380,7 +3380,7 @@
         <v>143</v>
       </c>
       <c r="L2" t="s">
-        <v>144</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -3388,10 +3388,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" t="s">
         <v>145</v>
-      </c>
-      <c r="C3" t="s">
-        <v>146</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>
@@ -3409,16 +3409,16 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J3" t="s">
         <v>142</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L3" t="s">
-        <v>149</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -3426,10 +3426,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
@@ -3447,16 +3447,16 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J4" t="s">
         <v>142</v>
       </c>
       <c r="K4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L4" t="s">
-        <v>154</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -3464,10 +3464,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -3479,22 +3479,22 @@
         <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L5" t="s">
-        <v>161</v>
+        <v>487</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -3502,10 +3502,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -3517,22 +3517,22 @@
         <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L6" t="s">
-        <v>166</v>
+        <v>488</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -3540,10 +3540,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>16</v>
@@ -3555,22 +3555,22 @@
         <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
       </c>
       <c r="I7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L7" t="s">
-        <v>171</v>
+        <v>489</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -3578,10 +3578,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
@@ -3593,22 +3593,22 @@
         <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J8" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="L8" t="s">
-        <v>178</v>
+        <v>490</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -3616,10 +3616,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>16</v>
@@ -3631,22 +3631,22 @@
         <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="J9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K9" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="L9" t="s">
-        <v>183</v>
+        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -3654,10 +3654,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
@@ -3669,22 +3669,22 @@
         <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="H10" t="s">
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="J10" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K10" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="L10" t="s">
-        <v>188</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -3721,7 +3721,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="15" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -3735,367 +3735,367 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -4126,7 +4126,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="3" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -4154,127 +4154,127 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -4284,22 +4284,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -4307,19 +4307,19 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -4327,19 +4327,19 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -4347,19 +4347,19 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -4367,19 +4367,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>135</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -4387,19 +4387,19 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -4407,19 +4407,19 @@
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -4427,19 +4427,19 @@
         <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -4447,19 +4447,19 @@
         <v>7</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -4467,19 +4467,19 @@
         <v>8</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -4487,19 +4487,19 @@
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -4507,19 +4507,19 @@
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -4527,19 +4527,19 @@
         <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -4547,24 +4547,24 @@
         <v>12</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="19" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -4574,22 +4574,22 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -4597,19 +4597,19 @@
         <v>19</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -4617,19 +4617,19 @@
         <v>26</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -4637,19 +4637,19 @@
         <v>32</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -4657,19 +4657,19 @@
         <v>38</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -4677,19 +4677,19 @@
         <v>45</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -4697,19 +4697,19 @@
         <v>53</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -4717,19 +4717,19 @@
         <v>59</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -4737,19 +4737,19 @@
         <v>73</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -4757,19 +4757,19 @@
         <v>87</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -4777,19 +4777,19 @@
         <v>105</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -4797,64 +4797,64 @@
         <v>138</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4867,147 +4867,147 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>136</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A60" s="12" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5020,107 +5020,107 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A69" s="10" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5133,107 +5133,107 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="11" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>